<commit_message>
Complete Milestone 2: Acquire initial assets, setup some FMOD events, and integrate those FMOD events
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Unity Projects\adventure-game\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B7158A-E68D-4317-9028-D775ECB3A60B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29C1DDA-96B8-4070-B52F-D5434CAB7205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6EA8544D-7128-4E6F-BE10-F5F759F1A5B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Events" sheetId="1" r:id="rId1"/>
+    <sheet name="Sources" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
   <si>
     <t>Event</t>
   </si>
@@ -140,9 +141,6 @@
     <t>GlassesDrop</t>
   </si>
   <si>
-    <t>Effect for collecting a glasses</t>
-  </si>
-  <si>
     <t>Glasses, or generic sounding picking up sound effect</t>
   </si>
   <si>
@@ -203,20 +201,110 @@
     <t>Several electronic beeping sounds, laser buzzing sound</t>
   </si>
   <si>
-    <t>Positive and Negative, and Win pop sound</t>
-  </si>
-  <si>
     <t>Incomplete</t>
   </si>
   <si>
     <t>Dialog</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>beep-*</t>
+  </si>
+  <si>
+    <t>Created from FL Studio</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>laser_sustained.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/ledhed2222/sounds/397280/</t>
+  </si>
+  <si>
+    <t>Assets Acquired</t>
+  </si>
+  <si>
+    <t>Crowd Exterior Large Size, City Voices, Footsteps, Distant Traffic Stereo .wav</t>
+  </si>
+  <si>
+    <t>https://sonniss.com/gameaudiogdc19/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/miastodzwiekow/sounds/122328/</t>
+  </si>
+  <si>
+    <t>argument ambience_130611.wav</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/passAirmangrace/sounds/340893/</t>
+  </si>
+  <si>
+    <t>MaleSnore_Raw_bip.wav</t>
+  </si>
+  <si>
+    <t>guitar_ac_fx_006.wav</t>
+  </si>
+  <si>
+    <t>button_002.wav</t>
+  </si>
+  <si>
+    <t>marimba_tone_007.wav</t>
+  </si>
+  <si>
+    <t>org_short_R_to_L_002.wav</t>
+  </si>
+  <si>
+    <t>S23_SFX_Footsteps_Gravel_Loafers_Loops_Walk_Normal.wav</t>
+  </si>
+  <si>
+    <t>S23_SFX_Footsteps_Metal_Boots_Loop_Jogging.wav</t>
+  </si>
+  <si>
+    <t>S23_SFX_Footsteps_Snow_Singles_Sequence.wav</t>
+  </si>
+  <si>
+    <t>Coins_Bottlecaps_Drop.wav</t>
+  </si>
+  <si>
+    <t>PRB216 Saker Falcon (Tosia) - Call, Squawk Screech Scream Cry, High Nervous - 8060 MF.wav</t>
+  </si>
+  <si>
+    <t>Glass,Plate Glass,Thick,Break,Topple,Schoeps.wav</t>
+  </si>
+  <si>
+    <t>Effect for collecting a pair of glasses</t>
+  </si>
+  <si>
+    <t>Water_Pouring_02.wav</t>
+  </si>
+  <si>
+    <t>Positive, Negative sounds</t>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Effect for winning the game</t>
+  </si>
+  <si>
+    <t>Win sfx</t>
+  </si>
+  <si>
+    <t>Implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +326,14 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -256,15 +352,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137DB1-84FE-4B50-A7A2-240641D04329}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -590,6 +689,7 @@
     <col min="3" max="3" width="29" customWidth="1"/>
     <col min="4" max="4" width="47.6640625" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" customWidth="1"/>
+    <col min="6" max="6" width="19.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -608,6 +708,9 @@
       <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -620,61 +723,61 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" t="s">
         <v>46</v>
-      </c>
-      <c r="B3" t="s">
-        <v>47</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
         <v>49</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>51</v>
-      </c>
       <c r="E4" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
       <c r="E5" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
@@ -688,10 +791,10 @@
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
       <c r="E6" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="F6" s="2"/>
     </row>
@@ -709,7 +812,7 @@
         <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -726,7 +829,7 @@
         <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -743,24 +846,24 @@
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
         <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E10" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -777,7 +880,7 @@
         <v>22</v>
       </c>
       <c r="E11" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -794,7 +897,7 @@
         <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -811,7 +914,7 @@
         <v>30</v>
       </c>
       <c r="E13" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -828,7 +931,7 @@
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -836,50 +939,67 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>35</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
         <v>37</v>
-      </c>
-      <c r="B16" t="s">
-        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
       </c>
       <c r="D16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B17" t="s">
         <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>41</v>
       </c>
       <c r="C17" t="s">
         <v>20</v>
       </c>
       <c r="D17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17" t="s">
-        <v>57</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -889,4 +1009,177 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8E5EE8-6CEC-463A-A887-2CEBB44CEDC8}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="79.109375" customWidth="1"/>
+    <col min="2" max="2" width="55.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>76</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>80</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>82</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{F93F5934-189E-45A8-B79A-6085FEF84FAB}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{B099165B-9B4D-4152-A247-7FD3D89CEB83}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{7388007E-FF67-41D1-824D-4CB8B6FBA579}"/>
+    <hyperlink ref="B6" r:id="rId4" xr:uid="{17C97B6D-2AC2-47AE-927A-8500C7B39985}"/>
+    <hyperlink ref="B7" r:id="rId5" xr:uid="{E787BB59-5925-413E-8C30-06E97ADBAD08}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{3256B96D-38C1-4B1C-9ECE-089A13F7FAF7}"/>
+    <hyperlink ref="B9" r:id="rId7" xr:uid="{4C871566-3E60-43B6-8121-6C57EBF0907C}"/>
+    <hyperlink ref="B10" r:id="rId8" xr:uid="{7CC23928-A9D9-4439-9546-6264579E3EDA}"/>
+    <hyperlink ref="B11" r:id="rId9" xr:uid="{DAD2BE9E-53C5-4738-9E07-A98B6C9EC3C9}"/>
+    <hyperlink ref="B12" r:id="rId10" xr:uid="{8D52E386-DFBF-4E9F-8FFD-4E74DADAD0F9}"/>
+    <hyperlink ref="B13" r:id="rId11" xr:uid="{E0118947-6AD3-4009-8FCA-0706911F166F}"/>
+    <hyperlink ref="B14" r:id="rId12" xr:uid="{2F9303E5-DA09-4B15-8663-ABF285490BD1}"/>
+    <hyperlink ref="B15" r:id="rId13" xr:uid="{1E42C466-6319-4EE3-B1BB-B65412BA397B}"/>
+    <hyperlink ref="B16" r:id="rId14" xr:uid="{CE4C4EA0-C17A-4594-BA16-CE9364D38F12}"/>
+    <hyperlink ref="B17" r:id="rId15" xr:uid="{D2A761C8-2E36-4203-8B9C-6409217B4E84}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implement more events and integrate into game
</commit_message>
<xml_diff>
--- a/documentation/AssetList.xlsx
+++ b/documentation/AssetList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repos\Unity Projects\adventure-game\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29C1DDA-96B8-4070-B52F-D5434CAB7205}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{894579EE-0A62-4032-B562-E668512FFC85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6EA8544D-7128-4E6F-BE10-F5F759F1A5B6}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="82">
   <si>
     <t>Event</t>
   </si>
@@ -45,21 +45,12 @@
     <t>Assets Required</t>
   </si>
   <si>
-    <t>SecurityRoomBG</t>
-  </si>
-  <si>
-    <t>Background music for the security room</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
     <t>Music</t>
   </si>
   <si>
-    <t>Security Room Background Track</t>
-  </si>
-  <si>
     <t>SecurityRoomAmbience</t>
   </si>
   <si>
@@ -81,9 +72,6 @@
     <t>Sounds for dialogue text appearing</t>
   </si>
   <si>
-    <t>MovementInterface</t>
-  </si>
-  <si>
     <t>Interface sound for clicking to move somewhere</t>
   </si>
   <si>
@@ -135,15 +123,9 @@
     <t>Sound Effect for glasses hitting ground</t>
   </si>
   <si>
-    <t>CollectGlasses</t>
-  </si>
-  <si>
     <t>GlassesDrop</t>
   </si>
   <si>
-    <t>Glasses, or generic sounding picking up sound effect</t>
-  </si>
-  <si>
     <t>CollectFish</t>
   </si>
   <si>
@@ -201,9 +183,6 @@
     <t>Several electronic beeping sounds, laser buzzing sound</t>
   </si>
   <si>
-    <t>Incomplete</t>
-  </si>
-  <si>
     <t>Dialog</t>
   </si>
   <si>
@@ -228,9 +207,6 @@
     <t>https://freesound.org/people/ledhed2222/sounds/397280/</t>
   </si>
   <si>
-    <t>Assets Acquired</t>
-  </si>
-  <si>
     <t>Crowd Exterior Large Size, City Voices, Footsteps, Distant Traffic Stereo .wav</t>
   </si>
   <si>
@@ -279,9 +255,6 @@
     <t>Glass,Plate Glass,Thick,Break,Topple,Schoeps.wav</t>
   </si>
   <si>
-    <t>Effect for collecting a pair of glasses</t>
-  </si>
-  <si>
     <t>Water_Pouring_02.wav</t>
   </si>
   <si>
@@ -298,6 +271,15 @@
   </si>
   <si>
     <t>Implemented</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/munyeca/sounds/348148/</t>
+  </si>
+  <si>
+    <t>Grinding Beans for Cold Brew Coffee</t>
+  </si>
+  <si>
+    <t>GroundClick</t>
   </si>
 </sst>
 </file>
@@ -676,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2137DB1-84FE-4B50-A7A2-240641D04329}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -700,238 +682,238 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D3" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>49</v>
       </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="E4" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
         <v>4</v>
       </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="C12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
-      </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
         <v>28</v>
       </c>
-      <c r="B13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>30</v>
-      </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
         <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D14" t="s">
         <v>32</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -939,72 +921,38 @@
         <v>33</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>34</v>
       </c>
       <c r="C15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
       </c>
       <c r="E15" t="s">
-        <v>55</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D16" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="E16" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>40</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" t="s">
-        <v>86</v>
-      </c>
-      <c r="E18" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F17">
-    <sortCondition ref="C2:C17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F15">
+    <sortCondition ref="C2:C15"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1013,10 +961,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E8E5EE8-6CEC-463A-A887-2CEBB44CEDC8}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1027,138 +975,146 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>66</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1178,8 +1134,9 @@
     <hyperlink ref="B15" r:id="rId13" xr:uid="{1E42C466-6319-4EE3-B1BB-B65412BA397B}"/>
     <hyperlink ref="B16" r:id="rId14" xr:uid="{CE4C4EA0-C17A-4594-BA16-CE9364D38F12}"/>
     <hyperlink ref="B17" r:id="rId15" xr:uid="{D2A761C8-2E36-4203-8B9C-6409217B4E84}"/>
+    <hyperlink ref="B18" r:id="rId16" xr:uid="{2CD5E558-C4B7-4613-837E-1FF7C3D16AD4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>